<commit_message>
Excel import works with JSON path columns
</commit_message>
<xml_diff>
--- a/docs/excel_import/sample.xlsx
+++ b/docs/excel_import/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thokrl/Documents/aws-ai-qna-bot/docs/excel_import/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thokrl/Documents/GitHub/aws-ai-qna-bot/docs/excel_import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53B024C-788E-3949-A8DD-0E686D21FE3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFE62DE-5446-2149-BC83-AEE0A2F3DA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67700" yWindow="4420" windowWidth="37380" windowHeight="17180" xr2:uid="{65063F85-4105-8F42-BAD0-641D55AA808E}"/>
+    <workbookView xWindow="69480" yWindow="5000" windowWidth="37860" windowHeight="20260" xr2:uid="{65063F85-4105-8F42-BAD0-641D55AA808E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
   <si>
     <t>qid</t>
   </si>
@@ -106,6 +106,18 @@
   </si>
   <si>
     <t>NoAnswerWarning</t>
+  </si>
+  <si>
+    <t>QnAYesNoBot</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>clientFilterValues</t>
+  </si>
+  <si>
+    <t>elicitResponse.responsebot_hook</t>
   </si>
 </sst>
 </file>
@@ -494,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654EBFE9-4F2B-8349-985B-01DDB193FC33}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,7 +523,7 @@
     <col min="13" max="13" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,8 +563,12 @@
       <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="N1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -605,6 +621,12 @@
       <c r="M2" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="N2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="175" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">

</xml_diff>